<commit_message>
externalize some messages and update code and centers data based on OEM spec
</commit_message>
<xml_diff>
--- a/etc/order.xlsx
+++ b/etc/order.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="4">
   <si>
     <t>ZONE</t>
   </si>
@@ -880,7 +880,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -941,16 +941,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
+    <row r="8" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="CiFvIuqvK6ZFMGHGgBL+9YFAIIZtAB3XvTVkCyl53QG9DXj1LCjtgQZqgdaNk38KAYlufGk6tRoL48hsdY8x2A==" saltValue="C3m42DCsSA0mz7+sdJN1Mw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="L3whFnalcNNxZHwEWoW1cPM88QIMx3vmyAQ2bNYJmpp1EbQYcyIM+ebJddFJjm9zvYp3CgciEGqZxiQNMA5R6g==" saltValue="bpSqoYIRj0I0tozLPMRxsg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
@@ -995,7 +988,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="QNiBB/frUXwBNcYBopnCVvkKMEDJ6Z5+1Y84GenS0Z+7DbMqkJitdp3ZaNjg4npNlOSasM5UFPYoQyZuCpdYIQ==" saltValue="I8VN6q8yd6l7Z7ugWEnzxA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="xlHWkHnhCImo7LpzcrTF1ZNNEt0ATDbdRqTwTrDuoObRuWs5pPNghWg+RcDaH0bxHv+usuUebTeorjCQfBqm5A==" saltValue="HjKz/hPxwq7b6GesvDoufg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>